<commit_message>
Streamlines and comments sections
</commit_message>
<xml_diff>
--- a/Data/LA_SWUDS_BalanceSheet.xlsx
+++ b/Data/LA_SWUDS_BalanceSheet.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23940" windowHeight="9690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23940" windowHeight="9690" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2000" sheetId="13" r:id="rId1"/>
+    <sheet name="2005" sheetId="14" r:id="rId2"/>
+    <sheet name="2010" sheetId="15" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="22">
   <si>
     <t>US Water Balance Sheet</t>
   </si>
@@ -651,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:V1048576"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,4 +918,546 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B40"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="16"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="18"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="20"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="20"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="20"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="19">
+        <f>SUM(B9:B11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="14"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="20"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="20"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="22">
+        <f>SUM(B14:B15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="23">
+        <f>B7+B12+B16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="13" t="str">
+        <f>B2</f>
+        <v>Aquaculture</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="15"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="24"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="19">
+        <f t="shared" ref="B24" si="0">SUM(B21:B23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="15"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="24"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="24"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="24"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="19">
+        <f t="shared" ref="B29" si="1">SUM(B26:B28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="21"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="16"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="16"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="18"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="23">
+        <f>B24+B29+B33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="25"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="23">
+        <f>B34-B17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="16"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="18"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="20"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="20"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="20"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="19">
+        <f>SUM(B9:B11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="14"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="20"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="20"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="22">
+        <f>SUM(B14:B15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="23">
+        <f>B7+B12+B16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="13" t="str">
+        <f>B2</f>
+        <v>Aquaculture</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="15"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="24"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="19">
+        <f t="shared" ref="B24" si="0">SUM(B21:B23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="15"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="24"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="24"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="24"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="19">
+        <f t="shared" ref="B29" si="1">SUM(B26:B28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="21"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="16"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="16"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="18"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="23">
+        <f>B24+B29+B33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="25"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="23">
+        <f>B34-B17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>